<commit_message>
edit average function to include all sample main
</commit_message>
<xml_diff>
--- a/storage/excel/sum911.xlsx
+++ b/storage/excel/sum911.xlsx
@@ -1923,22 +1923,22 @@
         <v>29</v>
       </c>
       <c r="E13" s="59">
-        <v>67233</v>
+        <v>64021.679346438</v>
       </c>
       <c r="F13" s="59">
-        <v>4.76</v>
+        <v>4.5284238744267</v>
       </c>
       <c r="G13" s="59">
-        <v>79026</v>
+        <v>80871.643099778</v>
       </c>
       <c r="H13" s="59">
-        <v>2.59</v>
+        <v>2.6486609124538</v>
       </c>
       <c r="I13" s="59">
-        <v>164026.21221318</v>
+        <v>14653179.662829</v>
       </c>
       <c r="J13" s="59">
-        <v>3.67</v>
+        <v>3.2802612676767</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1957,22 +1957,22 @@
         <v>29</v>
       </c>
       <c r="U13" s="59">
-        <v>2.5448275862069</v>
+        <v>0.11202970738324</v>
       </c>
       <c r="V13" s="59">
-        <v>0.30314909784168</v>
+        <v>0.00017248630915162</v>
       </c>
       <c r="W13" s="59">
-        <v>1.6655773420479</v>
+        <v>0.046346709218829</v>
       </c>
       <c r="X13" s="59">
-        <v>0.013619601216385</v>
+        <v>3.2962137196267E-5</v>
       </c>
       <c r="Y13" s="59">
-        <v>2.1052024641274</v>
+        <v>0.079188208301037</v>
       </c>
       <c r="Z13" s="59">
-        <v>0.15838434952903</v>
+        <v>0.00010272422317394</v>
       </c>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
@@ -1994,22 +1994,22 @@
         <v>30</v>
       </c>
       <c r="AL13" s="59">
-        <v>126.0985203232</v>
+        <v>126.05589319432</v>
       </c>
       <c r="AM13" s="59">
-        <v>10.74485491674</v>
+        <v>10.741222659088</v>
       </c>
       <c r="AN13" s="59">
-        <v>171.86231964988</v>
+        <v>171.87755282999</v>
       </c>
       <c r="AO13" s="59">
-        <v>14.644388257366</v>
+        <v>14.645686276644</v>
       </c>
       <c r="AP13" s="59">
-        <v>297.96083997307</v>
+        <v>297.93344602431</v>
       </c>
       <c r="AQ13" s="59">
-        <v>25.389243174106</v>
+        <v>25.386908935731</v>
       </c>
       <c r="AR13" s="18"/>
       <c r="AS13" s="18"/>
@@ -2028,22 +2028,22 @@
         <v>29</v>
       </c>
       <c r="BB13" s="59">
-        <v>2.5364061302682</v>
+        <v>0.11119704218074</v>
       </c>
       <c r="BC13" s="59">
-        <v>0.10039149272343</v>
+        <v>0.00011136377794092</v>
       </c>
       <c r="BD13" s="59">
-        <v>2.6056644880174</v>
+        <v>0.069826567055922</v>
       </c>
       <c r="BE13" s="59">
-        <v>0.040414306309758</v>
+        <v>5.4331619780551E-5</v>
       </c>
       <c r="BF13" s="59">
-        <v>2.5710353091428</v>
+        <v>0.09051180461833</v>
       </c>
       <c r="BG13" s="59">
-        <v>0.070402899516593</v>
+        <v>8.2847698860737E-5</v>
       </c>
       <c r="BH13" s="18"/>
       <c r="BI13" s="18"/>
@@ -2064,22 +2064,22 @@
         <v>32</v>
       </c>
       <c r="E14" s="59">
-        <v>245694</v>
+        <v>234223.50292334</v>
       </c>
       <c r="F14" s="59">
-        <v>17.38</v>
+        <v>16.567252115496</v>
       </c>
       <c r="G14" s="59">
-        <v>249652</v>
+        <v>255500.57220997</v>
       </c>
       <c r="H14" s="59">
-        <v>8.18</v>
+        <v>8.3680058025676</v>
       </c>
       <c r="I14" s="59">
-        <v>570781.82896824</v>
+        <v>49687085.569448</v>
       </c>
       <c r="J14" s="59">
-        <v>12.78</v>
+        <v>11.122952563712</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -2096,22 +2096,22 @@
         <v>32</v>
       </c>
       <c r="U14" s="59">
-        <v>3.7597494089835</v>
+        <v>0.62334563658678</v>
       </c>
       <c r="V14" s="59">
-        <v>0.0082625827430052</v>
+        <v>0.00055772720929879</v>
       </c>
       <c r="W14" s="59">
-        <v>3.1179166666667</v>
+        <v>0.26127202727207</v>
       </c>
       <c r="X14" s="59">
-        <v>0.0023850292219113</v>
+        <v>5.9913050515838E-5</v>
       </c>
       <c r="Y14" s="59">
-        <v>3.4388330378251</v>
+        <v>0.44230883192943</v>
       </c>
       <c r="Z14" s="59">
-        <v>0.0053238059824582</v>
+        <v>0.00030882012990731</v>
       </c>
       <c r="AA14" s="18"/>
       <c r="AB14" s="18"/>
@@ -2131,22 +2131,22 @@
         <v>30</v>
       </c>
       <c r="AL14" s="59">
-        <v>53.808433634663</v>
+        <v>53.816700705681</v>
       </c>
       <c r="AM14" s="59">
-        <v>4.5850166300096</v>
+        <v>4.5857210671311</v>
       </c>
       <c r="AN14" s="59">
-        <v>95.38401271732</v>
+        <v>95.459621202124</v>
       </c>
       <c r="AO14" s="59">
-        <v>8.1276717236428</v>
+        <v>8.134114322633</v>
       </c>
       <c r="AP14" s="59">
-        <v>149.19244635198</v>
+        <v>149.27632190781</v>
       </c>
       <c r="AQ14" s="59">
-        <v>12.712688353652</v>
+        <v>12.719835389764</v>
       </c>
       <c r="AR14" s="18"/>
       <c r="AS14" s="18"/>
@@ -2163,22 +2163,22 @@
         <v>32</v>
       </c>
       <c r="BB14" s="59">
-        <v>3.4108983451537</v>
+        <v>0.56495874297526</v>
       </c>
       <c r="BC14" s="59">
-        <v>0.015157002153607</v>
+        <v>0.00053489503253859</v>
       </c>
       <c r="BD14" s="59">
-        <v>3.0696875</v>
+        <v>0.25825524914775</v>
       </c>
       <c r="BE14" s="59">
-        <v>0.0089722067092417</v>
+        <v>9.8070443344129E-5</v>
       </c>
       <c r="BF14" s="59">
-        <v>3.2402929225768</v>
+        <v>0.4116069960615</v>
       </c>
       <c r="BG14" s="59">
-        <v>0.012064604431424</v>
+        <v>0.00031648273794136</v>
       </c>
       <c r="BH14" s="18"/>
       <c r="BI14" s="18"/>
@@ -2197,22 +2197,22 @@
         <v>33</v>
       </c>
       <c r="E15" s="59">
-        <v>1136482</v>
+        <v>1083506.6950793</v>
       </c>
       <c r="F15" s="59">
-        <v>80.39</v>
+        <v>76.639313997804</v>
       </c>
       <c r="G15" s="59">
-        <v>2318714</v>
+        <v>2373211.4723896</v>
       </c>
       <c r="H15" s="59">
-        <v>75.94</v>
+        <v>77.726038732139</v>
       </c>
       <c r="I15" s="59">
-        <v>3491636.4101651</v>
+        <v>345577093.61124</v>
       </c>
       <c r="J15" s="59">
-        <v>78.16</v>
+        <v>77.360899221402</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -2227,22 +2227,22 @@
         <v>33</v>
       </c>
       <c r="U15" s="59">
-        <v>4.2745512848575</v>
+        <v>3.2799454363413</v>
       </c>
       <c r="V15" s="59">
-        <v>0.0036029124890201</v>
+        <v>0.0028687052806054</v>
       </c>
       <c r="W15" s="59">
-        <v>3.7473757045938</v>
+        <v>2.9054901225792</v>
       </c>
       <c r="X15" s="59">
-        <v>0.00025160282779583</v>
+        <v>0.0004525482389531</v>
       </c>
       <c r="Y15" s="59">
-        <v>4.0109634947256</v>
+        <v>3.0927177794603</v>
       </c>
       <c r="Z15" s="59">
-        <v>0.001927257658408</v>
+        <v>0.0016606267597792</v>
       </c>
       <c r="AA15" s="18"/>
       <c r="AB15" s="18"/>
@@ -2260,22 +2260,22 @@
         <v>30</v>
       </c>
       <c r="AL15" s="59">
-        <v>89.679968832145</v>
+        <v>89.783366503334</v>
       </c>
       <c r="AM15" s="59">
-        <v>7.641630144187</v>
+        <v>7.6504406597491</v>
       </c>
       <c r="AN15" s="59">
-        <v>155.20923643282</v>
+        <v>155.2008090078</v>
       </c>
       <c r="AO15" s="59">
-        <v>13.225379036441</v>
+        <v>13.224660935555</v>
       </c>
       <c r="AP15" s="59">
-        <v>244.88920526496</v>
+        <v>244.98417551114</v>
       </c>
       <c r="AQ15" s="59">
-        <v>20.867009180628</v>
+        <v>20.875101595304</v>
       </c>
       <c r="AR15" s="18"/>
       <c r="AS15" s="18"/>
@@ -2290,22 +2290,22 @@
         <v>33</v>
       </c>
       <c r="BB15" s="59">
-        <v>2.759523355076</v>
+        <v>2.1145671507009</v>
       </c>
       <c r="BC15" s="59">
-        <v>0.0006198818678698</v>
+        <v>0.00074266492462434</v>
       </c>
       <c r="BD15" s="59">
-        <v>2.9973250751004</v>
+        <v>2.3129897787771</v>
       </c>
       <c r="BE15" s="59">
-        <v>0.00040973046629385</v>
+        <v>0.00038737251385758</v>
       </c>
       <c r="BF15" s="59">
-        <v>2.8784242150882</v>
+        <v>2.213778464739</v>
       </c>
       <c r="BG15" s="59">
-        <v>0.00051480616708183</v>
+        <v>0.00056501871924096</v>
       </c>
       <c r="BH15" s="18"/>
       <c r="BI15" s="18"/>
@@ -2324,22 +2324,22 @@
         <v>34</v>
       </c>
       <c r="E16" s="59">
-        <v>534854</v>
+        <v>510692.51084435</v>
       </c>
       <c r="F16" s="59">
-        <v>37.83</v>
+        <v>36.122641302241</v>
       </c>
       <c r="G16" s="59">
-        <v>1359617</v>
+        <v>1391642.134946</v>
       </c>
       <c r="H16" s="59">
-        <v>44.53</v>
+        <v>45.5782519765</v>
       </c>
       <c r="I16" s="59">
-        <v>1839565.3408282</v>
+        <v>189409276.94054</v>
       </c>
       <c r="J16" s="59">
-        <v>41.18</v>
+        <v>42.401166789949</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -2354,22 +2354,22 @@
         <v>34</v>
       </c>
       <c r="U16" s="59">
-        <v>3.5380185185185</v>
+        <v>1.2588422001163</v>
       </c>
       <c r="V16" s="59">
-        <v>0.0041048350950517</v>
+        <v>0.000286348277671</v>
       </c>
       <c r="W16" s="59">
-        <v>3.1526706337826</v>
+        <v>1.4082003974759</v>
       </c>
       <c r="X16" s="59">
-        <v>0.0018659760690854</v>
+        <v>0.00023281508130792</v>
       </c>
       <c r="Y16" s="59">
-        <v>3.3453445761506</v>
+        <v>1.3335212987961</v>
       </c>
       <c r="Z16" s="59">
-        <v>0.0029854055820686</v>
+        <v>0.00025958167948946</v>
       </c>
       <c r="AA16" s="18"/>
       <c r="AB16" s="18"/>
@@ -2387,22 +2387,22 @@
         <v>30</v>
       </c>
       <c r="AL16" s="59">
-        <v>38.521982526471</v>
+        <v>38.514895785964</v>
       </c>
       <c r="AM16" s="59">
-        <v>3.2824581310806</v>
+        <v>3.281854269922</v>
       </c>
       <c r="AN16" s="59">
-        <v>74.072160527957</v>
+        <v>74.090838444999</v>
       </c>
       <c r="AO16" s="59">
-        <v>6.3116887985872</v>
+        <v>6.3132803438984</v>
       </c>
       <c r="AP16" s="59">
-        <v>112.59414305443</v>
+        <v>112.60573423096</v>
       </c>
       <c r="AQ16" s="59">
-        <v>9.5941469296678</v>
+        <v>9.5951346138204</v>
       </c>
       <c r="AR16" s="18"/>
       <c r="AS16" s="18"/>
@@ -2417,22 +2417,22 @@
         <v>34</v>
       </c>
       <c r="BB16" s="59">
-        <v>2.7605560846561</v>
+        <v>1.0057497254699</v>
       </c>
       <c r="BC16" s="59">
-        <v>0.0019411221664003</v>
+        <v>0.00087525143760146</v>
       </c>
       <c r="BD16" s="59">
-        <v>2.8832735876111</v>
+        <v>1.3062711017625</v>
       </c>
       <c r="BE16" s="59">
-        <v>0.0005222648804287</v>
+        <v>0.00016381105636436</v>
       </c>
       <c r="BF16" s="59">
-        <v>2.8219148361336</v>
+        <v>1.1560104136162</v>
       </c>
       <c r="BG16" s="59">
-        <v>0.0012316935234145</v>
+        <v>0.00051953124698291</v>
       </c>
       <c r="BH16" s="18"/>
       <c r="BI16" s="18"/>
@@ -2453,22 +2453,22 @@
         <v>29</v>
       </c>
       <c r="E17" s="59">
-        <v>574391</v>
+        <v>547657.08000322</v>
       </c>
       <c r="F17" s="59">
-        <v>40.63</v>
+        <v>38.737243718106</v>
       </c>
       <c r="G17" s="59">
-        <v>1181807</v>
+        <v>1209530.2549106</v>
       </c>
       <c r="H17" s="59">
-        <v>38.71</v>
+        <v>39.613829839704</v>
       </c>
       <c r="I17" s="59">
-        <v>1771956.7520328</v>
+        <v>175642326.85088</v>
       </c>
       <c r="J17" s="59">
-        <v>39.67</v>
+        <v>39.319296902847</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -2485,22 +2485,22 @@
         <v>29</v>
       </c>
       <c r="U17" s="59">
-        <v>3.9649898063201</v>
+        <v>1.5352552289904</v>
       </c>
       <c r="V17" s="59">
-        <v>0.006985575893986</v>
+        <v>0.00067248535069573</v>
       </c>
       <c r="W17" s="59">
-        <v>3.0125363892611</v>
+        <v>1.1949900166824</v>
       </c>
       <c r="X17" s="59">
-        <v>0.0018556043220079</v>
+        <v>0.00040713742427301</v>
       </c>
       <c r="Y17" s="59">
-        <v>3.4887630977906</v>
+        <v>1.3651226228364</v>
       </c>
       <c r="Z17" s="59">
-        <v>0.0044205901079969</v>
+        <v>0.00053981138748437</v>
       </c>
       <c r="AA17" s="18"/>
       <c r="AB17" s="18"/>
@@ -2520,22 +2520,22 @@
         <v>30</v>
       </c>
       <c r="AL17" s="59">
-        <v>39.77653982543</v>
+        <v>39.835549404338</v>
       </c>
       <c r="AM17" s="59">
-        <v>3.3893589585249</v>
+        <v>3.3943871647436</v>
       </c>
       <c r="AN17" s="59">
-        <v>70.751112731621</v>
+        <v>70.75955575598</v>
       </c>
       <c r="AO17" s="59">
-        <v>6.0287023158614</v>
+        <v>6.0294217459671</v>
       </c>
       <c r="AP17" s="59">
-        <v>110.52765255705</v>
+        <v>110.59510516032</v>
       </c>
       <c r="AQ17" s="59">
-        <v>9.4180612743863</v>
+        <v>9.4238089107107</v>
       </c>
       <c r="AR17" s="18"/>
       <c r="AS17" s="18"/>
@@ -2552,22 +2552,22 @@
         <v>29</v>
       </c>
       <c r="BB17" s="59">
-        <v>2.7708639143731</v>
+        <v>1.0733230185389</v>
       </c>
       <c r="BC17" s="59">
-        <v>0.0039421102341754</v>
+        <v>0.00092169305384869</v>
       </c>
       <c r="BD17" s="59">
-        <v>2.7134665680884</v>
+        <v>1.0770363269747</v>
       </c>
       <c r="BE17" s="59">
-        <v>0.00092533805557302</v>
+        <v>0.00028855152834813</v>
       </c>
       <c r="BF17" s="59">
-        <v>2.7421652412307</v>
+        <v>1.0751796727568</v>
       </c>
       <c r="BG17" s="59">
-        <v>0.0024337241448742</v>
+        <v>0.00060512229109841</v>
       </c>
       <c r="BH17" s="18"/>
       <c r="BI17" s="18"/>
@@ -2588,22 +2588,22 @@
         <v>29</v>
       </c>
       <c r="E18" s="59">
-        <v>54776</v>
+        <v>52240.004082617</v>
       </c>
       <c r="F18" s="59">
-        <v>3.87</v>
+        <v>3.6950746075835</v>
       </c>
       <c r="G18" s="59">
-        <v>66454</v>
+        <v>68005.134546085</v>
       </c>
       <c r="H18" s="59">
-        <v>2.18</v>
+        <v>2.2272645245521</v>
       </c>
       <c r="I18" s="59">
-        <v>135149.51662881</v>
+        <v>12152453.873068</v>
       </c>
       <c r="J18" s="59">
-        <v>3.03</v>
+        <v>2.7204487124507</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -2620,22 +2620,22 @@
         <v>29</v>
       </c>
       <c r="U18" s="59">
-        <v>7.6953636363636</v>
+        <v>0.28857535688909</v>
       </c>
       <c r="V18" s="59">
-        <v>3.0347529900083</v>
+        <v>0.0024797607520841</v>
       </c>
       <c r="W18" s="59">
-        <v>4.0621118012422</v>
+        <v>0.093899377674621</v>
       </c>
       <c r="X18" s="59">
-        <v>0.077498976761879</v>
+        <v>8.2506238231905E-5</v>
       </c>
       <c r="Y18" s="59">
-        <v>5.8787377188029</v>
+        <v>0.19123736728186</v>
       </c>
       <c r="Z18" s="59">
-        <v>1.5561259833851</v>
+        <v>0.001281133495158</v>
       </c>
       <c r="AA18" s="18"/>
       <c r="AB18" s="18"/>
@@ -2655,22 +2655,22 @@
         <v>30</v>
       </c>
       <c r="AL18" s="59">
-        <v>27.663456104381</v>
+        <v>27.671122378722</v>
       </c>
       <c r="AM18" s="59">
-        <v>2.3572030946543</v>
+        <v>2.3578563378909</v>
       </c>
       <c r="AN18" s="59">
-        <v>43.27796144222</v>
+        <v>43.404628646441</v>
       </c>
       <c r="AO18" s="59">
-        <v>3.6877150944915</v>
+        <v>3.6985084069632</v>
       </c>
       <c r="AP18" s="59">
-        <v>70.9414175466</v>
+        <v>71.075751025163</v>
       </c>
       <c r="AQ18" s="59">
-        <v>6.0449181891458</v>
+        <v>6.0563647448541</v>
       </c>
       <c r="AR18" s="18"/>
       <c r="AS18" s="18"/>
@@ -2687,22 +2687,22 @@
         <v>29</v>
       </c>
       <c r="BB18" s="59">
-        <v>2.7708639143731</v>
+        <v>1.0733230185389</v>
       </c>
       <c r="BC18" s="59">
-        <v>0.0039421102341754</v>
+        <v>0.00092169305384869</v>
       </c>
       <c r="BD18" s="59">
-        <v>2.7134665680884</v>
+        <v>1.0770363269747</v>
       </c>
       <c r="BE18" s="59">
-        <v>0.00092533805557302</v>
+        <v>0.00028855152834813</v>
       </c>
       <c r="BF18" s="59">
-        <v>2.7421652412307</v>
+        <v>1.0751796727568</v>
       </c>
       <c r="BG18" s="59">
-        <v>0.0024337241448742</v>
+        <v>0.00060512229109841</v>
       </c>
       <c r="BH18" s="18"/>
       <c r="BI18" s="18"/>
@@ -2725,22 +2725,22 @@
         <v>29</v>
       </c>
       <c r="E19" s="59">
-        <v>21189</v>
+        <v>20224.328847529</v>
       </c>
       <c r="F19" s="59">
-        <v>1.5</v>
+        <v>1.4305206382017</v>
       </c>
       <c r="G19" s="59">
-        <v>21552</v>
+        <v>22062.338765457</v>
       </c>
       <c r="H19" s="59">
-        <v>0.71</v>
+        <v>0.72257285848988</v>
       </c>
       <c r="I19" s="59">
-        <v>49240.878758222</v>
+        <v>4290374.2309521</v>
       </c>
       <c r="J19" s="59">
-        <v>1.1</v>
+        <v>0.96044331247304</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -2759,22 +2759,22 @@
         <v>29</v>
       </c>
       <c r="U19" s="59">
-        <v>1.6908571428571</v>
+        <v>0.025039241651056</v>
       </c>
       <c r="V19" s="59">
-        <v>0.1190823784289</v>
+        <v>0.00031333498779066</v>
       </c>
       <c r="W19" s="59">
-        <v>1.3125</v>
+        <v>0.0090315340538188</v>
       </c>
       <c r="X19" s="59">
-        <v>0.25176091147678</v>
+        <v>4.9106547248952E-6</v>
       </c>
       <c r="Y19" s="59">
-        <v>1.5016785714286</v>
+        <v>0.017035387852437</v>
       </c>
       <c r="Z19" s="59">
-        <v>0.18542164495284</v>
+        <v>0.00015912282125778</v>
       </c>
       <c r="AA19" s="18"/>
       <c r="AB19" s="18"/>
@@ -2796,22 +2796,22 @@
         <v>30</v>
       </c>
       <c r="AL19" s="59">
-        <v>149.23961533913</v>
+        <v>151.04666571961</v>
       </c>
       <c r="AM19" s="59">
-        <v>12.716707623047</v>
+        <v>12.870686385968</v>
       </c>
       <c r="AN19" s="59">
-        <v>196.41203572567</v>
+        <v>195.10819412682</v>
       </c>
       <c r="AO19" s="59">
-        <v>16.736269564185</v>
+        <v>16.625169221546</v>
       </c>
       <c r="AP19" s="59">
-        <v>345.65165106481</v>
+        <v>346.15485984643</v>
       </c>
       <c r="AQ19" s="59">
-        <v>29.452977187232</v>
+        <v>29.495855607514</v>
       </c>
       <c r="AR19" s="18"/>
       <c r="AS19" s="18"/>
@@ -2830,22 +2830,22 @@
         <v>29</v>
       </c>
       <c r="BB19" s="59">
-        <v>3.4125714285714</v>
+        <v>0.052474465473807</v>
       </c>
       <c r="BC19" s="59">
-        <v>0.54706532416325</v>
+        <v>0.0009363151627737</v>
       </c>
       <c r="BD19" s="59">
-        <v>2.4375</v>
+        <v>0.016858988902589</v>
       </c>
       <c r="BE19" s="59">
-        <v>0.46772374431075</v>
+        <v>1.4564471976064E-5</v>
       </c>
       <c r="BF19" s="59">
-        <v>2.9250357142857</v>
+        <v>0.034666727188198</v>
       </c>
       <c r="BG19" s="59">
-        <v>0.507394534237</v>
+        <v>0.00047543981737488</v>
       </c>
       <c r="BH19" s="18"/>
       <c r="BI19" s="18"/>
@@ -2866,22 +2866,22 @@
         <v>32</v>
       </c>
       <c r="E20" s="59">
-        <v>29999</v>
+        <v>28654.087599587</v>
       </c>
       <c r="F20" s="59">
-        <v>2.12</v>
+        <v>2.0267799237775</v>
       </c>
       <c r="G20" s="59">
-        <v>61066</v>
+        <v>62502.943904583</v>
       </c>
       <c r="H20" s="59">
-        <v>2</v>
+        <v>2.0470599840429</v>
       </c>
       <c r="I20" s="59">
-        <v>92064.384120534</v>
+        <v>9113935.4618398</v>
       </c>
       <c r="J20" s="59">
-        <v>2.06</v>
+        <v>2.0402458837938</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -2898,22 +2898,22 @@
         <v>32</v>
       </c>
       <c r="U20" s="59">
-        <v>1.17</v>
+        <v>0.025041521865513</v>
       </c>
       <c r="V20" s="59">
-        <v>0.085419134691406</v>
+        <v>8.3412319482699E-5</v>
       </c>
       <c r="W20" s="59">
-        <v>1.5350877192982</v>
+        <v>0.031912172336259</v>
       </c>
       <c r="X20" s="59">
-        <v>0.026160187673656</v>
+        <v>3.772924430951E-5</v>
       </c>
       <c r="Y20" s="59">
-        <v>1.3525438596491</v>
+        <v>0.028476847100886</v>
       </c>
       <c r="Z20" s="59">
-        <v>0.055789661182531</v>
+        <v>6.0570781896104E-5</v>
       </c>
       <c r="AA20" s="18"/>
       <c r="AB20" s="18"/>
@@ -2933,22 +2933,22 @@
         <v>30</v>
       </c>
       <c r="AL20" s="59">
-        <v>40.156534713874</v>
+        <v>40.015347494752</v>
       </c>
       <c r="AM20" s="59">
-        <v>3.4217383229692</v>
+        <v>3.4097077600278</v>
       </c>
       <c r="AN20" s="59">
-        <v>93.193546681821</v>
+        <v>92.819834057596</v>
       </c>
       <c r="AO20" s="59">
-        <v>7.941022112758</v>
+        <v>7.9091780600478</v>
       </c>
       <c r="AP20" s="59">
-        <v>133.3500813957</v>
+        <v>132.83518155235</v>
       </c>
       <c r="AQ20" s="59">
-        <v>11.362760435727</v>
+        <v>11.318885820076</v>
       </c>
       <c r="AR20" s="18"/>
       <c r="AS20" s="18"/>
@@ -2965,22 +2965,22 @@
         <v>32</v>
       </c>
       <c r="BB20" s="59">
-        <v>3.8133333333333</v>
+        <v>0.084076435630773</v>
       </c>
       <c r="BC20" s="59">
-        <v>0.31422366361741</v>
+        <v>0.00031881631121423</v>
       </c>
       <c r="BD20" s="59">
-        <v>2.2298245614035</v>
+        <v>0.046363002828752</v>
       </c>
       <c r="BE20" s="59">
-        <v>0.021290361381434</v>
+        <v>2.2381550802796E-5</v>
       </c>
       <c r="BF20" s="59">
-        <v>3.0215789473684</v>
+        <v>0.065219719229762</v>
       </c>
       <c r="BG20" s="59">
-        <v>0.16775701249942</v>
+        <v>0.00017059893100851</v>
       </c>
       <c r="BH20" s="18"/>
       <c r="BI20" s="18"/>
@@ -2999,22 +2999,22 @@
         <v>33</v>
       </c>
       <c r="E21" s="59">
-        <v>305890</v>
+        <v>291499.44104338</v>
       </c>
       <c r="F21" s="59">
-        <v>21.64</v>
+        <v>20.618531748595</v>
       </c>
       <c r="G21" s="59">
-        <v>466975</v>
+        <v>477943.99154995</v>
       </c>
       <c r="H21" s="59">
-        <v>15.29</v>
+        <v>15.653343004279</v>
       </c>
       <c r="I21" s="59">
-        <v>824857.09865322</v>
+        <v>77377128.335499</v>
       </c>
       <c r="J21" s="59">
-        <v>18.47</v>
+        <v>17.321646422369</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -3029,22 +3029,22 @@
         <v>33</v>
       </c>
       <c r="U21" s="59">
-        <v>1.9491803278689</v>
+        <v>0.40282775014534</v>
       </c>
       <c r="V21" s="59">
-        <v>0.0014371820790784</v>
+        <v>0.00069574753945809</v>
       </c>
       <c r="W21" s="59">
-        <v>1.7297777777778</v>
+        <v>0.27092534126351</v>
       </c>
       <c r="X21" s="59">
-        <v>0.00097727330633719</v>
+        <v>8.2216087975888E-5</v>
       </c>
       <c r="Y21" s="59">
-        <v>1.8394790528233</v>
+        <v>0.33687654570442</v>
       </c>
       <c r="Z21" s="59">
-        <v>0.0012072276927078</v>
+        <v>0.00038898181371699</v>
       </c>
       <c r="AA21" s="18"/>
       <c r="AB21" s="18"/>
@@ -3062,22 +3062,22 @@
         <v>30</v>
       </c>
       <c r="AL21" s="59">
-        <v>78.045621362914</v>
+        <v>78.409882133461</v>
       </c>
       <c r="AM21" s="59">
-        <v>6.6502673963339</v>
+        <v>6.6813060565922</v>
       </c>
       <c r="AN21" s="59">
-        <v>145.01053501191</v>
+        <v>144.98936278946</v>
       </c>
       <c r="AO21" s="59">
-        <v>12.356347688365</v>
+        <v>12.354543603289</v>
       </c>
       <c r="AP21" s="59">
-        <v>223.05615637483</v>
+        <v>223.39924492292</v>
       </c>
       <c r="AQ21" s="59">
-        <v>19.006615084699</v>
+        <v>19.035849659882</v>
       </c>
       <c r="AR21" s="18"/>
       <c r="AS21" s="18"/>
@@ -3092,22 +3092,22 @@
         <v>33</v>
       </c>
       <c r="BB21" s="59">
-        <v>2.6634699453552</v>
+        <v>0.54706526387184</v>
       </c>
       <c r="BC21" s="59">
-        <v>0.0081642209198156</v>
+        <v>0.00065828158569729</v>
       </c>
       <c r="BD21" s="59">
-        <v>3.6798814814815</v>
+        <v>0.57409067672445</v>
       </c>
       <c r="BE21" s="59">
-        <v>0.0032213262806697</v>
+        <v>0.00022857327053705</v>
       </c>
       <c r="BF21" s="59">
-        <v>3.1716757134183</v>
+        <v>0.56057797029815</v>
       </c>
       <c r="BG21" s="59">
-        <v>0.0056927736002426</v>
+        <v>0.00044342742811717</v>
       </c>
       <c r="BH21" s="18"/>
       <c r="BI21" s="18"/>
@@ -3126,22 +3126,22 @@
         <v>34</v>
       </c>
       <c r="E22" s="59">
-        <v>155459</v>
+        <v>148299.92461953</v>
       </c>
       <c r="F22" s="59">
-        <v>11</v>
+        <v>10.489648601512</v>
       </c>
       <c r="G22" s="59">
-        <v>301738</v>
+        <v>308811.51277418</v>
       </c>
       <c r="H22" s="59">
-        <v>9.88</v>
+        <v>10.114014651483</v>
       </c>
       <c r="I22" s="59">
-        <v>466326.56954644</v>
+        <v>45743885.44891</v>
       </c>
       <c r="J22" s="59">
-        <v>10.44</v>
+        <v>10.240227658693</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -3156,22 +3156,22 @@
         <v>34</v>
       </c>
       <c r="U22" s="59">
-        <v>1.6790303030303</v>
+        <v>0.1740060138234</v>
       </c>
       <c r="V22" s="59">
-        <v>0.0019282463840392</v>
+        <v>0.00021276913755565</v>
       </c>
       <c r="W22" s="59">
-        <v>1.6232954545455</v>
+        <v>0.16494631754551</v>
       </c>
       <c r="X22" s="59">
-        <v>0.0037024170217562</v>
+        <v>2.9310008013092E-5</v>
       </c>
       <c r="Y22" s="59">
-        <v>1.6511628787879</v>
+        <v>0.16947616568446</v>
       </c>
       <c r="Z22" s="59">
-        <v>0.0028153317028977</v>
+        <v>0.00012103957278437</v>
       </c>
       <c r="AA22" s="18"/>
       <c r="AB22" s="18"/>
@@ -3189,22 +3189,22 @@
         <v>30</v>
       </c>
       <c r="AL22" s="59">
-        <v>37.385712642544</v>
+        <v>37.525744112731</v>
       </c>
       <c r="AM22" s="59">
-        <v>3.1856365742712</v>
+        <v>3.1975686558458</v>
       </c>
       <c r="AN22" s="59">
-        <v>58.673686035603</v>
+        <v>58.62079643708</v>
       </c>
       <c r="AO22" s="59">
-        <v>4.9995847870938</v>
+        <v>4.9950780644036</v>
       </c>
       <c r="AP22" s="59">
-        <v>96.059398678147</v>
+        <v>96.146540549811</v>
       </c>
       <c r="AQ22" s="59">
-        <v>8.1852213613649</v>
+        <v>8.1926467202494</v>
       </c>
       <c r="AR22" s="18"/>
       <c r="AS22" s="18"/>
@@ -3219,22 +3219,22 @@
         <v>34</v>
       </c>
       <c r="BB22" s="59">
-        <v>3.5008484848485</v>
+        <v>0.36713656094568</v>
       </c>
       <c r="BC22" s="59">
-        <v>0.017478067991792</v>
+        <v>0.00048579142426178</v>
       </c>
       <c r="BD22" s="59">
-        <v>3.43125</v>
+        <v>0.34825781968521</v>
       </c>
       <c r="BE22" s="59">
-        <v>0.0044118683170081</v>
+        <v>0.00023020846394379</v>
       </c>
       <c r="BF22" s="59">
-        <v>3.4660492424242</v>
+        <v>0.35769719031544</v>
       </c>
       <c r="BG22" s="59">
-        <v>0.0109449681544</v>
+        <v>0.00035799994410279</v>
       </c>
       <c r="BH22" s="18"/>
       <c r="BI22" s="18"/>
@@ -3255,22 +3255,22 @@
         <v>29</v>
       </c>
       <c r="E23" s="59">
-        <v>137896</v>
+        <v>131430.73599168</v>
       </c>
       <c r="F23" s="59">
-        <v>9.75</v>
+        <v>9.2964459660229</v>
       </c>
       <c r="G23" s="59">
-        <v>237079</v>
+        <v>242666.59206309</v>
       </c>
       <c r="H23" s="59">
-        <v>7.76</v>
+        <v>7.947674766084</v>
       </c>
       <c r="I23" s="59">
-        <v>391280.75613114</v>
+        <v>37527296.925705</v>
       </c>
       <c r="J23" s="59">
-        <v>8.76</v>
+        <v>8.4008618892635</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -3287,22 +3287,22 @@
         <v>29</v>
       </c>
       <c r="U23" s="59">
-        <v>2.4897222222222</v>
+        <v>0.23122227892255</v>
       </c>
       <c r="V23" s="59">
-        <v>0.020547032886406</v>
+        <v>0.00021708081178716</v>
       </c>
       <c r="W23" s="59">
-        <v>1.6623931623932</v>
+        <v>0.12883960832668</v>
       </c>
       <c r="X23" s="59">
-        <v>0.005988710016527</v>
+        <v>3.8229357213274E-5</v>
       </c>
       <c r="Y23" s="59">
-        <v>2.0760576923077</v>
+        <v>0.18003094362462</v>
       </c>
       <c r="Z23" s="59">
-        <v>0.013267871451467</v>
+        <v>0.00012765508450022</v>
       </c>
       <c r="AA23" s="18"/>
       <c r="AB23" s="18"/>
@@ -3322,22 +3322,22 @@
         <v>30</v>
       </c>
       <c r="AL23" s="59">
-        <v>47.433229633251</v>
+        <v>47.680387123738</v>
       </c>
       <c r="AM23" s="59">
-        <v>4.0417854970493</v>
+        <v>4.0628457868137</v>
       </c>
       <c r="AN23" s="59">
-        <v>72.597190767484</v>
+        <v>72.340554279735</v>
       </c>
       <c r="AO23" s="59">
-        <v>6.1860066252973</v>
+        <v>6.1641386301762</v>
       </c>
       <c r="AP23" s="59">
-        <v>120.03042040073</v>
+        <v>120.02094140347</v>
       </c>
       <c r="AQ23" s="59">
-        <v>10.227792122347</v>
+        <v>10.22698441699</v>
       </c>
       <c r="AR23" s="18"/>
       <c r="AS23" s="18"/>
@@ -3354,22 +3354,22 @@
         <v>29</v>
       </c>
       <c r="BB23" s="59">
-        <v>3.15125</v>
+        <v>0.29260415024869</v>
       </c>
       <c r="BC23" s="59">
-        <v>0.043754669678741</v>
+        <v>0.00027206378154065</v>
       </c>
       <c r="BD23" s="59">
-        <v>2.8906695156695</v>
+        <v>0.22547338797418</v>
       </c>
       <c r="BE23" s="59">
-        <v>0.0055170558494693</v>
+        <v>7.3651858804946E-5</v>
       </c>
       <c r="BF23" s="59">
-        <v>3.0209597578348</v>
+        <v>0.25903876911144</v>
       </c>
       <c r="BG23" s="59">
-        <v>0.024635862764105</v>
+        <v>0.0001728578201728</v>
       </c>
       <c r="BH23" s="18"/>
       <c r="BI23" s="18"/>
@@ -3390,22 +3390,22 @@
         <v>29</v>
       </c>
       <c r="E24" s="59">
-        <v>24737</v>
+        <v>23592.363898857</v>
       </c>
       <c r="F24" s="59">
-        <v>1.75</v>
+        <v>1.6687507266972</v>
       </c>
       <c r="G24" s="59">
-        <v>21552</v>
+        <v>22054.685022679</v>
       </c>
       <c r="H24" s="59">
-        <v>0.71</v>
+        <v>0.722322187568</v>
       </c>
       <c r="I24" s="59">
-        <v>54846.155554937</v>
+        <v>4647199.2681954</v>
       </c>
       <c r="J24" s="59">
-        <v>1.23</v>
+        <v>1.0403221767154</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -3422,22 +3422,22 @@
         <v>29</v>
       </c>
       <c r="U24" s="59">
-        <v>5.1106666666667</v>
+        <v>0.084612725276145</v>
       </c>
       <c r="V24" s="59">
-        <v>0.56862437110233</v>
+        <v>0.00035937452256057</v>
       </c>
       <c r="W24" s="59">
-        <v>3.625</v>
+        <v>0.027085828679191</v>
       </c>
       <c r="X24" s="59">
-        <v>0.77587701299485</v>
+        <v>2.5559528386435E-5</v>
       </c>
       <c r="Y24" s="59">
-        <v>4.3678333333333</v>
+        <v>0.055849276977668</v>
       </c>
       <c r="Z24" s="59">
-        <v>0.67225069204859</v>
+        <v>0.0001924670254735</v>
       </c>
       <c r="AA24" s="18"/>
       <c r="AB24" s="18"/>
@@ -3457,22 +3457,22 @@
         <v>30</v>
       </c>
       <c r="AL24" s="59">
-        <v>27.265399552037</v>
+        <v>27.538191147353</v>
       </c>
       <c r="AM24" s="59">
-        <v>2.3232846958291</v>
+        <v>2.346529267666</v>
       </c>
       <c r="AN24" s="59">
-        <v>26.2678710393</v>
+        <v>26.339510687589</v>
       </c>
       <c r="AO24" s="59">
-        <v>2.2382852912588</v>
+        <v>2.2443897056895</v>
       </c>
       <c r="AP24" s="59">
-        <v>53.533270591337</v>
+        <v>53.877701834942</v>
       </c>
       <c r="AQ24" s="59">
-        <v>4.5615699870878</v>
+        <v>4.5909189733554</v>
       </c>
       <c r="AR24" s="18"/>
       <c r="AS24" s="18"/>
@@ -3489,22 +3489,22 @@
         <v>29</v>
       </c>
       <c r="BB24" s="59">
-        <v>2.0366666666667</v>
+        <v>0.033970589755184</v>
       </c>
       <c r="BC24" s="59">
-        <v>0.090590787623717</v>
+        <v>0.00014937094706819</v>
       </c>
       <c r="BD24" s="59">
-        <v>1.71875</v>
+        <v>0.012339775150504</v>
       </c>
       <c r="BE24" s="59">
-        <v>0.34315429174673</v>
+        <v>9.5751001795045E-6</v>
       </c>
       <c r="BF24" s="59">
-        <v>1.8777083333333</v>
+        <v>0.023155182452844</v>
       </c>
       <c r="BG24" s="59">
-        <v>0.21687253968522</v>
+        <v>7.9473023623846E-5</v>
       </c>
       <c r="BH24" s="18"/>
       <c r="BI24" s="18"/>

</xml_diff>

<commit_message>
update sum and average according to revised calculation
</commit_message>
<xml_diff>
--- a/storage/excel/sum911.xlsx
+++ b/storage/excel/sum911.xlsx
@@ -1935,7 +1935,7 @@
         <v>2.6486609124538</v>
       </c>
       <c r="I13" s="59">
-        <v>14653179.662829</v>
+        <v>146531.79662829</v>
       </c>
       <c r="J13" s="59">
         <v>3.2802612676767</v>
@@ -1960,19 +1960,19 @@
         <v>0.11202970738324</v>
       </c>
       <c r="V13" s="59">
-        <v>0.00017248630915162</v>
+        <v>0.00017514738276494</v>
       </c>
       <c r="W13" s="59">
         <v>0.046346709218829</v>
       </c>
       <c r="X13" s="59">
-        <v>3.2962137196267E-5</v>
+        <v>3.2949416841522E-5</v>
       </c>
       <c r="Y13" s="59">
         <v>0.079188208301037</v>
       </c>
       <c r="Z13" s="59">
-        <v>0.00010272422317394</v>
+        <v>0.00010404839980323</v>
       </c>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
@@ -2031,19 +2031,19 @@
         <v>0.11119704218074</v>
       </c>
       <c r="BC13" s="59">
-        <v>0.00011136377794092</v>
+        <v>0.00010762372349109</v>
       </c>
       <c r="BD13" s="59">
         <v>0.069826567055922</v>
       </c>
       <c r="BE13" s="59">
-        <v>5.4331619780551E-5</v>
+        <v>5.4449172933301E-5</v>
       </c>
       <c r="BF13" s="59">
         <v>0.09051180461833</v>
       </c>
       <c r="BG13" s="59">
-        <v>8.2847698860737E-5</v>
+        <v>8.1036448212197E-5</v>
       </c>
       <c r="BH13" s="18"/>
       <c r="BI13" s="18"/>
@@ -2076,7 +2076,7 @@
         <v>8.3680058025676</v>
       </c>
       <c r="I14" s="59">
-        <v>49687085.569448</v>
+        <v>496870.85569448</v>
       </c>
       <c r="J14" s="59">
         <v>11.122952563712</v>
@@ -2099,19 +2099,19 @@
         <v>0.62334563658678</v>
       </c>
       <c r="V14" s="59">
-        <v>0.00055772720929879</v>
+        <v>0.00061406214394432</v>
       </c>
       <c r="W14" s="59">
         <v>0.26127202727207</v>
       </c>
       <c r="X14" s="59">
-        <v>5.9913050515838E-5</v>
+        <v>5.9157575372947E-5</v>
       </c>
       <c r="Y14" s="59">
         <v>0.44230883192943</v>
       </c>
       <c r="Z14" s="59">
-        <v>0.00030882012990731</v>
+        <v>0.00033660985965864</v>
       </c>
       <c r="AA14" s="18"/>
       <c r="AB14" s="18"/>
@@ -2166,19 +2166,19 @@
         <v>0.56495874297526</v>
       </c>
       <c r="BC14" s="59">
-        <v>0.00053489503253859</v>
+        <v>0.00056631026953784</v>
       </c>
       <c r="BD14" s="59">
         <v>0.25825524914775</v>
       </c>
       <c r="BE14" s="59">
-        <v>9.8070443344129E-5</v>
+        <v>9.8388675745353E-5</v>
       </c>
       <c r="BF14" s="59">
         <v>0.4116069960615</v>
       </c>
       <c r="BG14" s="59">
-        <v>0.00031648273794136</v>
+        <v>0.00033234947264159</v>
       </c>
       <c r="BH14" s="18"/>
       <c r="BI14" s="18"/>
@@ -2209,7 +2209,7 @@
         <v>77.726038732139</v>
       </c>
       <c r="I15" s="59">
-        <v>345577093.61124</v>
+        <v>3455770.9361124</v>
       </c>
       <c r="J15" s="59">
         <v>77.360899221402</v>
@@ -2230,19 +2230,19 @@
         <v>3.2799454363413</v>
       </c>
       <c r="V15" s="59">
-        <v>0.0028687052806054</v>
+        <v>0.0028471808990454</v>
       </c>
       <c r="W15" s="59">
         <v>2.9054901225792</v>
       </c>
       <c r="X15" s="59">
-        <v>0.0004525482389531</v>
+        <v>0.00044685505209112</v>
       </c>
       <c r="Y15" s="59">
         <v>3.0927177794603</v>
       </c>
       <c r="Z15" s="59">
-        <v>0.0016606267597792</v>
+        <v>0.0016470179755683</v>
       </c>
       <c r="AA15" s="18"/>
       <c r="AB15" s="18"/>
@@ -2293,19 +2293,19 @@
         <v>2.1145671507009</v>
       </c>
       <c r="BC15" s="59">
-        <v>0.00074266492462434</v>
+        <v>0.00073662388676653</v>
       </c>
       <c r="BD15" s="59">
         <v>2.3129897787771</v>
       </c>
       <c r="BE15" s="59">
-        <v>0.00038737251385758</v>
+        <v>0.00038566555538187</v>
       </c>
       <c r="BF15" s="59">
         <v>2.213778464739</v>
       </c>
       <c r="BG15" s="59">
-        <v>0.00056501871924096</v>
+        <v>0.0005611447210742</v>
       </c>
       <c r="BH15" s="18"/>
       <c r="BI15" s="18"/>
@@ -2336,7 +2336,7 @@
         <v>45.5782519765</v>
       </c>
       <c r="I16" s="59">
-        <v>189409276.94054</v>
+        <v>1894092.7694054</v>
       </c>
       <c r="J16" s="59">
         <v>42.401166789949</v>
@@ -2357,19 +2357,19 @@
         <v>1.2588422001163</v>
       </c>
       <c r="V16" s="59">
-        <v>0.000286348277671</v>
+        <v>0.00031927634645803</v>
       </c>
       <c r="W16" s="59">
         <v>1.4082003974759</v>
       </c>
       <c r="X16" s="59">
-        <v>0.00023281508130792</v>
+        <v>0.00025174669218715</v>
       </c>
       <c r="Y16" s="59">
         <v>1.3335212987961</v>
       </c>
       <c r="Z16" s="59">
-        <v>0.00025958167948946</v>
+        <v>0.00028551151932259</v>
       </c>
       <c r="AA16" s="18"/>
       <c r="AB16" s="18"/>
@@ -2420,19 +2420,19 @@
         <v>1.0057497254699</v>
       </c>
       <c r="BC16" s="59">
-        <v>0.00087525143760146</v>
+        <v>0.00099366690198437</v>
       </c>
       <c r="BD16" s="59">
         <v>1.3062711017625</v>
       </c>
       <c r="BE16" s="59">
-        <v>0.00016381105636436</v>
+        <v>0.00016139587383638</v>
       </c>
       <c r="BF16" s="59">
         <v>1.1560104136162</v>
       </c>
       <c r="BG16" s="59">
-        <v>0.00051953124698291</v>
+        <v>0.00057753138791038</v>
       </c>
       <c r="BH16" s="18"/>
       <c r="BI16" s="18"/>
@@ -2465,7 +2465,7 @@
         <v>39.613829839704</v>
       </c>
       <c r="I17" s="59">
-        <v>175642326.85088</v>
+        <v>1756423.2685088</v>
       </c>
       <c r="J17" s="59">
         <v>39.319296902847</v>
@@ -2488,19 +2488,19 @@
         <v>1.5352552289904</v>
       </c>
       <c r="V17" s="59">
-        <v>0.00067248535069573</v>
+        <v>0.00079653611333741</v>
       </c>
       <c r="W17" s="59">
         <v>1.1949900166824</v>
       </c>
       <c r="X17" s="59">
-        <v>0.00040713742427301</v>
+        <v>0.00041296619359969</v>
       </c>
       <c r="Y17" s="59">
         <v>1.3651226228364</v>
       </c>
       <c r="Z17" s="59">
-        <v>0.00053981138748437</v>
+        <v>0.00060475115346855</v>
       </c>
       <c r="AA17" s="18"/>
       <c r="AB17" s="18"/>
@@ -2555,19 +2555,19 @@
         <v>1.0733230185389</v>
       </c>
       <c r="BC17" s="59">
-        <v>0.00092169305384869</v>
+        <v>0.00098165508203396</v>
       </c>
       <c r="BD17" s="59">
         <v>1.0770363269747</v>
       </c>
       <c r="BE17" s="59">
-        <v>0.00028855152834813</v>
+        <v>0.00028572417174936</v>
       </c>
       <c r="BF17" s="59">
         <v>1.0751796727568</v>
       </c>
       <c r="BG17" s="59">
-        <v>0.00060512229109841</v>
+        <v>0.00063368962689166</v>
       </c>
       <c r="BH17" s="18"/>
       <c r="BI17" s="18"/>
@@ -2600,7 +2600,7 @@
         <v>2.2272645245521</v>
       </c>
       <c r="I18" s="59">
-        <v>12152453.873068</v>
+        <v>121524.53873068</v>
       </c>
       <c r="J18" s="59">
         <v>2.7204487124507</v>
@@ -2623,19 +2623,19 @@
         <v>0.28857535688909</v>
       </c>
       <c r="V18" s="59">
-        <v>0.0024797607520841</v>
+        <v>0.0024791463296305</v>
       </c>
       <c r="W18" s="59">
         <v>0.093899377674621</v>
       </c>
       <c r="X18" s="59">
-        <v>8.2506238231905E-5</v>
+        <v>8.1732261327908E-5</v>
       </c>
       <c r="Y18" s="59">
         <v>0.19123736728186</v>
       </c>
       <c r="Z18" s="59">
-        <v>0.001281133495158</v>
+        <v>0.0012804392954792</v>
       </c>
       <c r="AA18" s="18"/>
       <c r="AB18" s="18"/>
@@ -2687,22 +2687,22 @@
         <v>29</v>
       </c>
       <c r="BB18" s="59">
-        <v>1.0733230185389</v>
+        <v>0.093578276597119</v>
       </c>
       <c r="BC18" s="59">
-        <v>0.00092169305384869</v>
+        <v>0.00017844791591164</v>
       </c>
       <c r="BD18" s="59">
-        <v>1.0770363269747</v>
+        <v>0.048159408138101</v>
       </c>
       <c r="BE18" s="59">
-        <v>0.00028855152834813</v>
+        <v>2.5983743476353E-5</v>
       </c>
       <c r="BF18" s="59">
-        <v>1.0751796727568</v>
+        <v>0.07086884236761</v>
       </c>
       <c r="BG18" s="59">
-        <v>0.00060512229109841</v>
+        <v>0.000102215829694</v>
       </c>
       <c r="BH18" s="18"/>
       <c r="BI18" s="18"/>
@@ -2737,7 +2737,7 @@
         <v>0.72257285848988</v>
       </c>
       <c r="I19" s="59">
-        <v>4290374.2309521</v>
+        <v>42903.742309521</v>
       </c>
       <c r="J19" s="59">
         <v>0.96044331247304</v>
@@ -2762,19 +2762,19 @@
         <v>0.025039241651056</v>
       </c>
       <c r="V19" s="59">
-        <v>0.00031333498779066</v>
+        <v>0.00031311216205559</v>
       </c>
       <c r="W19" s="59">
         <v>0.0090315340538188</v>
       </c>
       <c r="X19" s="59">
-        <v>4.9106547248952E-6</v>
+        <v>4.9700816999396E-6</v>
       </c>
       <c r="Y19" s="59">
         <v>0.017035387852437</v>
       </c>
       <c r="Z19" s="59">
-        <v>0.00015912282125778</v>
+        <v>0.00015904112187777</v>
       </c>
       <c r="AA19" s="18"/>
       <c r="AB19" s="18"/>
@@ -2833,19 +2833,19 @@
         <v>0.052474465473807</v>
       </c>
       <c r="BC19" s="59">
-        <v>0.0009363151627737</v>
+        <v>0.0009360391777865</v>
       </c>
       <c r="BD19" s="59">
         <v>0.016858988902589</v>
       </c>
       <c r="BE19" s="59">
-        <v>1.4564471976064E-5</v>
+        <v>1.4675772868101E-5</v>
       </c>
       <c r="BF19" s="59">
         <v>0.034666727188198</v>
       </c>
       <c r="BG19" s="59">
-        <v>0.00047543981737488</v>
+        <v>0.0004753574753273</v>
       </c>
       <c r="BH19" s="18"/>
       <c r="BI19" s="18"/>
@@ -2878,7 +2878,7 @@
         <v>2.0470599840429</v>
       </c>
       <c r="I20" s="59">
-        <v>9113935.4618398</v>
+        <v>91139.354618398</v>
       </c>
       <c r="J20" s="59">
         <v>2.0402458837938</v>
@@ -2901,19 +2901,19 @@
         <v>0.025041521865513</v>
       </c>
       <c r="V20" s="59">
-        <v>8.3412319482699E-5</v>
+        <v>8.5471390050154E-5</v>
       </c>
       <c r="W20" s="59">
         <v>0.031912172336259</v>
       </c>
       <c r="X20" s="59">
-        <v>3.772924430951E-5</v>
+        <v>3.7922166643766E-5</v>
       </c>
       <c r="Y20" s="59">
         <v>0.028476847100886</v>
       </c>
       <c r="Z20" s="59">
-        <v>6.0570781896104E-5</v>
+        <v>6.169677834696E-5</v>
       </c>
       <c r="AA20" s="18"/>
       <c r="AB20" s="18"/>
@@ -2968,19 +2968,19 @@
         <v>0.084076435630773</v>
       </c>
       <c r="BC20" s="59">
-        <v>0.00031881631121423</v>
+        <v>0.00032787496410973</v>
       </c>
       <c r="BD20" s="59">
         <v>0.046363002828752</v>
       </c>
       <c r="BE20" s="59">
-        <v>2.2381550802796E-5</v>
+        <v>2.3020046069941E-5</v>
       </c>
       <c r="BF20" s="59">
         <v>0.065219719229762</v>
       </c>
       <c r="BG20" s="59">
-        <v>0.00017059893100851</v>
+        <v>0.00017544750508984</v>
       </c>
       <c r="BH20" s="18"/>
       <c r="BI20" s="18"/>
@@ -3011,7 +3011,7 @@
         <v>15.653343004279</v>
       </c>
       <c r="I21" s="59">
-        <v>77377128.335499</v>
+        <v>773771.28335499</v>
       </c>
       <c r="J21" s="59">
         <v>17.321646422369</v>
@@ -3032,19 +3032,19 @@
         <v>0.40282775014534</v>
       </c>
       <c r="V21" s="59">
-        <v>0.00069574753945809</v>
+        <v>0.00068930648224643</v>
       </c>
       <c r="W21" s="59">
         <v>0.27092534126351</v>
       </c>
       <c r="X21" s="59">
-        <v>8.2216087975888E-5</v>
+        <v>8.2221652269679E-5</v>
       </c>
       <c r="Y21" s="59">
         <v>0.33687654570442</v>
       </c>
       <c r="Z21" s="59">
-        <v>0.00038898181371699</v>
+        <v>0.00038576406725805</v>
       </c>
       <c r="AA21" s="18"/>
       <c r="AB21" s="18"/>
@@ -3095,19 +3095,19 @@
         <v>0.54706526387184</v>
       </c>
       <c r="BC21" s="59">
-        <v>0.00065828158569729</v>
+        <v>0.00064693380821351</v>
       </c>
       <c r="BD21" s="59">
         <v>0.57409067672445</v>
       </c>
       <c r="BE21" s="59">
-        <v>0.00022857327053705</v>
+        <v>0.00023003772909532</v>
       </c>
       <c r="BF21" s="59">
         <v>0.56057797029815</v>
       </c>
       <c r="BG21" s="59">
-        <v>0.00044342742811717</v>
+        <v>0.00043848576865441</v>
       </c>
       <c r="BH21" s="18"/>
       <c r="BI21" s="18"/>
@@ -3138,7 +3138,7 @@
         <v>10.114014651483</v>
       </c>
       <c r="I22" s="59">
-        <v>45743885.44891</v>
+        <v>457438.8544891</v>
       </c>
       <c r="J22" s="59">
         <v>10.240227658693</v>
@@ -3159,19 +3159,19 @@
         <v>0.1740060138234</v>
       </c>
       <c r="V22" s="59">
-        <v>0.00021276913755565</v>
+        <v>0.00021934841407676</v>
       </c>
       <c r="W22" s="59">
         <v>0.16494631754551</v>
       </c>
       <c r="X22" s="59">
-        <v>2.9310008013092E-5</v>
+        <v>3.1561798919809E-5</v>
       </c>
       <c r="Y22" s="59">
         <v>0.16947616568446</v>
       </c>
       <c r="Z22" s="59">
-        <v>0.00012103957278437</v>
+        <v>0.00012545510649828</v>
       </c>
       <c r="AA22" s="18"/>
       <c r="AB22" s="18"/>
@@ -3222,19 +3222,19 @@
         <v>0.36713656094568</v>
       </c>
       <c r="BC22" s="59">
-        <v>0.00048579142426178</v>
+        <v>0.00051960973387959</v>
       </c>
       <c r="BD22" s="59">
         <v>0.34825781968521</v>
       </c>
       <c r="BE22" s="59">
-        <v>0.00023020846394379</v>
+        <v>0.00023109931148739</v>
       </c>
       <c r="BF22" s="59">
         <v>0.35769719031544</v>
       </c>
       <c r="BG22" s="59">
-        <v>0.00035799994410279</v>
+        <v>0.00037535452268349</v>
       </c>
       <c r="BH22" s="18"/>
       <c r="BI22" s="18"/>
@@ -3267,7 +3267,7 @@
         <v>7.947674766084</v>
       </c>
       <c r="I23" s="59">
-        <v>37527296.925705</v>
+        <v>375272.96925705</v>
       </c>
       <c r="J23" s="59">
         <v>8.4008618892635</v>
@@ -3290,19 +3290,19 @@
         <v>0.23122227892255</v>
       </c>
       <c r="V23" s="59">
-        <v>0.00021708081178716</v>
+        <v>0.00020984782310985</v>
       </c>
       <c r="W23" s="59">
         <v>0.12883960832668</v>
       </c>
       <c r="X23" s="59">
-        <v>3.8229357213274E-5</v>
+        <v>3.8115212342259E-5</v>
       </c>
       <c r="Y23" s="59">
         <v>0.18003094362462</v>
       </c>
       <c r="Z23" s="59">
-        <v>0.00012765508450022</v>
+        <v>0.00012398151772605</v>
       </c>
       <c r="AA23" s="18"/>
       <c r="AB23" s="18"/>
@@ -3357,19 +3357,19 @@
         <v>0.29260415024869</v>
       </c>
       <c r="BC23" s="59">
-        <v>0.00027206378154065</v>
+        <v>0.00026197451907916</v>
       </c>
       <c r="BD23" s="59">
         <v>0.22547338797418</v>
       </c>
       <c r="BE23" s="59">
-        <v>7.3651858804946E-5</v>
+        <v>7.3621997054271E-5</v>
       </c>
       <c r="BF23" s="59">
         <v>0.25903876911144</v>
       </c>
       <c r="BG23" s="59">
-        <v>0.0001728578201728</v>
+        <v>0.00016779825806671</v>
       </c>
       <c r="BH23" s="18"/>
       <c r="BI23" s="18"/>
@@ -3402,7 +3402,7 @@
         <v>0.722322187568</v>
       </c>
       <c r="I24" s="59">
-        <v>4647199.2681954</v>
+        <v>46471.992681954</v>
       </c>
       <c r="J24" s="59">
         <v>1.0403221767154</v>
@@ -3425,19 +3425,19 @@
         <v>0.084612725276145</v>
       </c>
       <c r="V24" s="59">
-        <v>0.00035937452256057</v>
+        <v>0.00035901545523597</v>
       </c>
       <c r="W24" s="59">
         <v>0.027085828679191</v>
       </c>
       <c r="X24" s="59">
-        <v>2.5559528386435E-5</v>
+        <v>2.5587407323813E-5</v>
       </c>
       <c r="Y24" s="59">
         <v>0.055849276977668</v>
       </c>
       <c r="Z24" s="59">
-        <v>0.0001924670254735</v>
+        <v>0.00019230143127989</v>
       </c>
       <c r="AA24" s="18"/>
       <c r="AB24" s="18"/>
@@ -3492,19 +3492,19 @@
         <v>0.033970589755184</v>
       </c>
       <c r="BC24" s="59">
-        <v>0.00014937094706819</v>
+        <v>0.00014904332933008</v>
       </c>
       <c r="BD24" s="59">
         <v>0.012339775150504</v>
       </c>
       <c r="BE24" s="59">
-        <v>9.5751001795045E-6</v>
+        <v>9.6068755493027E-6</v>
       </c>
       <c r="BF24" s="59">
         <v>0.023155182452844</v>
       </c>
       <c r="BG24" s="59">
-        <v>7.9473023623846E-5</v>
+        <v>7.9325102439689E-5</v>
       </c>
       <c r="BH24" s="18"/>
       <c r="BI24" s="18"/>

</xml_diff>